<commit_message>
Problem solving with weighted data
</commit_message>
<xml_diff>
--- a/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/sege_sum_w-raw-ss-lookup-tabbed.xlsx
+++ b/OUTPUT-FILES/NORMS/TODE_8.27.21_fornorms/sege_sum_w-raw-ss-lookup-tabbed.xlsx
@@ -356,7 +356,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -574,78 +574,6 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>130</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -653,7 +581,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -871,78 +799,6 @@
         <v>130</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>130</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -950,7 +806,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1168,78 +1024,6 @@
         <v>128</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>130</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1247,7 +1031,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1465,78 +1249,6 @@
         <v>122</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>130</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1544,7 +1256,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -1762,78 +1474,6 @@
         <v>117</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>130</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1841,7 +1481,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:B26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2059,78 +1699,6 @@
         <v>113</v>
       </c>
     </row>
-    <row r="27">
-      <c r="A27">
-        <v>26</v>
-      </c>
-      <c r="B27">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28">
-        <v>27</v>
-      </c>
-      <c r="B28">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30">
-        <v>29</v>
-      </c>
-      <c r="B30">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31">
-        <v>30</v>
-      </c>
-      <c r="B31">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32">
-        <v>31</v>
-      </c>
-      <c r="B32">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33">
-        <v>32</v>
-      </c>
-      <c r="B33">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34">
-        <v>33</v>
-      </c>
-      <c r="B34">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35">
-        <v>34</v>
-      </c>
-      <c r="B35">
-        <v>130</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>